<commit_message>
raw data and images try 1
</commit_message>
<xml_diff>
--- a/Cake_club_scores_sheet_2024.xlsx
+++ b/Cake_club_scores_sheet_2024.xlsx
@@ -58,7 +58,7 @@
     <t xml:space="preserve">30-10-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 17</t>
+    <t xml:space="preserve">Baker17</t>
   </si>
   <si>
     <t xml:space="preserve">Basque cheese cake</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">23-10-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 16</t>
+    <t xml:space="preserve">Baker16</t>
   </si>
   <si>
     <t xml:space="preserve">Carrot cake with lime frosting</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">28-08-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 8</t>
+    <t xml:space="preserve">Baker8</t>
   </si>
   <si>
     <t xml:space="preserve">Chocolate dream cake</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">04-09-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 9</t>
+    <t xml:space="preserve">Baker9</t>
   </si>
   <si>
     <t xml:space="preserve">Biscoff cheese cake</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">14-08-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 6</t>
+    <t xml:space="preserve">Baker6</t>
   </si>
   <si>
     <t xml:space="preserve">Apple pie with vanilla ice cream</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">16-10-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 15</t>
+    <t xml:space="preserve">Baker15</t>
   </si>
   <si>
     <t xml:space="preserve">Swiss Rolls</t>
@@ -151,13 +151,13 @@
     <t xml:space="preserve">21-08-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 7</t>
+    <t xml:space="preserve">Baker7</t>
   </si>
   <si>
     <t xml:space="preserve">04-12-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 20</t>
+    <t xml:space="preserve">Baker20</t>
   </si>
   <si>
     <t xml:space="preserve">Mjuk pepparkake</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">19-06-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 3</t>
+    <t xml:space="preserve">Baker3</t>
   </si>
   <si>
     <t xml:space="preserve">Czech honey cake, medovnik</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">25-09-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 12</t>
+    <t xml:space="preserve">Baker12</t>
   </si>
   <si>
     <t xml:space="preserve">Apple-oat cake (tray)</t>
@@ -193,7 +193,7 @@
     <t xml:space="preserve">18-09-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 11</t>
+    <t xml:space="preserve">Baker11</t>
   </si>
   <si>
     <t xml:space="preserve">Lemon Merengue pie</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">07-08-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 5</t>
+    <t xml:space="preserve">Baker5</t>
   </si>
   <si>
     <t xml:space="preserve">Lemon Merengue berry pie</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">27-11-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 19</t>
+    <t xml:space="preserve">Baker19</t>
   </si>
   <si>
     <t xml:space="preserve">Tarragon Basque cheese cake</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">09-10-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 14</t>
+    <t xml:space="preserve">Baker14</t>
   </si>
   <si>
     <t xml:space="preserve">Tiramisu-Brownie</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">26-06-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 4</t>
+    <t xml:space="preserve">Baker4</t>
   </si>
   <si>
     <t xml:space="preserve">Strawberry-Sponge-Cake</t>
@@ -247,7 +247,7 @@
     <t xml:space="preserve">12-06-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 2</t>
+    <t xml:space="preserve">Baker2</t>
   </si>
   <si>
     <t xml:space="preserve">Rhubarb-Crumble-Cheesecake</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">02-10-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 13</t>
+    <t xml:space="preserve">Baker13</t>
   </si>
   <si>
     <t xml:space="preserve">Cherry-Chocolate cake with vanilla creme</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">11-09-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 10</t>
+    <t xml:space="preserve">Baker10</t>
   </si>
   <si>
     <t xml:space="preserve">Linzer Torte</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">05-06-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 1</t>
+    <t xml:space="preserve">Baker1</t>
   </si>
   <si>
     <t xml:space="preserve">Drømmekage</t>
@@ -295,7 +295,7 @@
     <t xml:space="preserve">13-11-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 18</t>
+    <t xml:space="preserve">Baker18</t>
   </si>
   <si>
     <t xml:space="preserve">Nougat mousse bought</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">11-12-2024</t>
   </si>
   <si>
-    <t xml:space="preserve">Baker 21</t>
+    <t xml:space="preserve">Baker21</t>
   </si>
   <si>
     <t xml:space="preserve">Saffron bun</t>
@@ -345,12 +345,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="12">
@@ -464,56 +470,68 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,7 +544,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -538,6 +556,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
@@ -745,790 +771,790 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="9.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="36.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="49.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="25.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5" t="n">
+      <c r="I2" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" s="8" t="n">
         <v>9.22727272727273</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="E3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="8" t="n">
+      <c r="H3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="11" t="n">
         <v>14</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="9" t="n">
+      <c r="K3" s="12" t="n">
         <v>9.18181818181818</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="8" t="n">
+      <c r="H4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="9" t="n">
+      <c r="K4" s="12" t="n">
         <v>8.83333333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="11" t="n">
         <v>29</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="9" t="n">
+      <c r="K5" s="12" t="n">
         <v>8.8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="8" t="n">
+      <c r="H6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="12" t="n">
         <v>8.7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="8" t="n">
+      <c r="H7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="11" t="n">
         <v>12</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="9" t="n">
+      <c r="K7" s="12" t="n">
         <v>8.69230769230769</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="8" t="n">
+      <c r="H8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="11" t="n">
         <v>20</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="9" t="n">
+      <c r="K8" s="12" t="n">
         <v>8.625</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="8" t="n">
+      <c r="H9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="11" t="n">
         <v>4</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="9" t="n">
+      <c r="K9" s="12" t="n">
         <v>8.625</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="8" t="n">
+      <c r="H10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="11" t="n">
         <v>17</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="12" t="n">
         <v>8.54545454545455</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="H11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="9" t="n">
+      <c r="K11" s="12" t="n">
         <v>8.53333333333333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="8" t="n">
+      <c r="H12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="11" t="n">
         <v>19</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="12" t="n">
         <v>8.45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="8" t="n">
+      <c r="H13" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="11" t="n">
         <v>24</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="9" t="n">
+      <c r="K13" s="12" t="n">
         <v>8.375</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="E14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="11" t="n">
         <v>7</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="9" t="n">
+      <c r="K14" s="12" t="n">
         <v>8.16666666666667</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="8" t="n">
+      <c r="H15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="K15" s="9" t="n">
+      <c r="K15" s="12" t="n">
         <v>8.125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="E16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="8" t="n">
+      <c r="H16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="11" t="n">
         <v>26</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="K16" s="9" t="n">
+      <c r="K16" s="12" t="n">
         <v>8.08333333333333</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="E17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="I17" s="11" t="n">
         <v>16</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="K17" s="9" t="n">
+      <c r="K17" s="12" t="n">
         <v>8.03571428571429</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="8" t="n">
+      <c r="H18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="11" t="n">
         <v>11</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="9" t="n">
+      <c r="K18" s="12" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="J19" s="8" t="s">
+      <c r="H19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="J19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="K19" s="9" t="n">
+      <c r="K19" s="12" t="n">
         <v>7.83333333333333</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="8" t="s">
+      <c r="E20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="8" t="n">
+      <c r="H20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="11" t="n">
         <v>18</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="12" t="n">
         <v>7.76666666666667</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="8" t="n">
+      <c r="H21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="K21" s="9" t="n">
+      <c r="K21" s="12" t="n">
         <v>7.26923076923077</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="11" t="s">
+      <c r="E22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="11" t="n">
+      <c r="H22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="14" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="12" t="n">
+      <c r="K22" s="15" t="n">
         <v>6.5</v>
       </c>
     </row>

</xml_diff>